<commit_message>
Fix NLI skipping some topics/activities (3/?)
</commit_message>
<xml_diff>
--- a/results/nli-cv/cv_results-AppleSupport-inbound.xlsx
+++ b/results/nli-cv/cv_results-AppleSupport-inbound.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="128">
   <si>
     <t>Header</t>
   </si>
@@ -58,6 +58,15 @@
     <t>Mac</t>
   </si>
   <si>
+    <t>iCloud</t>
+  </si>
+  <si>
+    <t>iTunes</t>
+  </si>
+  <si>
+    <t>Refund</t>
+  </si>
+  <si>
     <t>This example is iphone</t>
   </si>
   <si>
@@ -269,6 +278,126 @@
   </si>
   <si>
     <t>The customer asks about Mac</t>
+  </si>
+  <si>
+    <t>This example is icloud</t>
+  </si>
+  <si>
+    <t>This example is iCloud</t>
+  </si>
+  <si>
+    <t>This example is about icloud</t>
+  </si>
+  <si>
+    <t>This example is about iCloud</t>
+  </si>
+  <si>
+    <t>The example is icloud</t>
+  </si>
+  <si>
+    <t>The example is iCloud</t>
+  </si>
+  <si>
+    <t>The example is about icloud</t>
+  </si>
+  <si>
+    <t>The example is about iCloud</t>
+  </si>
+  <si>
+    <t>The sentence is icloud</t>
+  </si>
+  <si>
+    <t>The sentence is iCloud</t>
+  </si>
+  <si>
+    <t>The sentence is about icloud</t>
+  </si>
+  <si>
+    <t>The sentence is about iCloud</t>
+  </si>
+  <si>
+    <t>The customer asks about icloud</t>
+  </si>
+  <si>
+    <t>The customer asks about iCloud</t>
+  </si>
+  <si>
+    <t>This example is itunes</t>
+  </si>
+  <si>
+    <t>This example is iTunes</t>
+  </si>
+  <si>
+    <t>This example is about itunes</t>
+  </si>
+  <si>
+    <t>This example is about iTunes</t>
+  </si>
+  <si>
+    <t>The example is itunes</t>
+  </si>
+  <si>
+    <t>The example is iTunes</t>
+  </si>
+  <si>
+    <t>The example is about itunes</t>
+  </si>
+  <si>
+    <t>The example is about iTunes</t>
+  </si>
+  <si>
+    <t>The sentence is itunes</t>
+  </si>
+  <si>
+    <t>The sentence is iTunes</t>
+  </si>
+  <si>
+    <t>The sentence is about itunes</t>
+  </si>
+  <si>
+    <t>The sentence is about iTunes</t>
+  </si>
+  <si>
+    <t>The customer asks about itunes</t>
+  </si>
+  <si>
+    <t>The customer asks about iTunes</t>
+  </si>
+  <si>
+    <t>This example is refund</t>
+  </si>
+  <si>
+    <t>This example is about refund</t>
+  </si>
+  <si>
+    <t>This example is about a refund</t>
+  </si>
+  <si>
+    <t>The example is refund</t>
+  </si>
+  <si>
+    <t>The example is about refund</t>
+  </si>
+  <si>
+    <t>The example is about a refund</t>
+  </si>
+  <si>
+    <t>The sentence is refund</t>
+  </si>
+  <si>
+    <t>The sentence is about refund</t>
+  </si>
+  <si>
+    <t>The sentence is about a refund</t>
+  </si>
+  <si>
+    <t>The customer asks about refund</t>
+  </si>
+  <si>
+    <t>The customer asks about a refund</t>
+  </si>
+  <si>
+    <t>The customer wants a refund</t>
   </si>
 </sst>
 </file>
@@ -626,7 +755,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -666,7 +795,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>0.7999999999999999</v>
@@ -695,7 +824,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>0.82</v>
@@ -724,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>0.76</v>
@@ -753,7 +882,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>0.8799999999999999</v>
@@ -782,7 +911,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>0.9099999999999999</v>
@@ -811,7 +940,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7">
         <v>0.85</v>
@@ -840,7 +969,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D8">
         <v>0.86</v>
@@ -869,7 +998,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <v>0.9399999999999998</v>
@@ -898,7 +1027,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>0.7</v>
@@ -927,7 +1056,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11">
         <v>0.73</v>
@@ -956,7 +1085,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D12">
         <v>0.9199999999999999</v>
@@ -985,7 +1114,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>0.97</v>
@@ -1014,7 +1143,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D14">
         <v>0.96</v>
@@ -1043,7 +1172,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>0.95</v>
@@ -1072,7 +1201,7 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D16">
         <v>0.76</v>
@@ -1101,7 +1230,7 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D17">
         <v>0.8699999999999999</v>
@@ -1130,7 +1259,7 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D18">
         <v>0.96</v>
@@ -1159,7 +1288,7 @@
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D19">
         <v>0.9299999999999999</v>
@@ -1188,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D20">
         <v>0.9299999999999999</v>
@@ -1217,7 +1346,7 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D21">
         <v>0.983</v>
@@ -1246,7 +1375,7 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D22">
         <v>0.86</v>
@@ -1275,7 +1404,7 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D23">
         <v>0.9099999999999999</v>
@@ -1304,7 +1433,7 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <v>0.993</v>
@@ -1333,7 +1462,7 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D25">
         <v>0.99</v>
@@ -1362,7 +1491,7 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D26">
         <v>0.998</v>
@@ -1391,7 +1520,7 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D27">
         <v>0.9949999999999999</v>
@@ -1420,7 +1549,7 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D28">
         <v>0.7899999999999999</v>
@@ -1449,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D29">
         <v>0.82</v>
@@ -1478,7 +1607,7 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D30">
         <v>0.73</v>
@@ -1507,7 +1636,7 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D31">
         <v>0.8699999999999999</v>
@@ -1536,7 +1665,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D32">
         <v>0.85</v>
@@ -1565,7 +1694,7 @@
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D33">
         <v>0.85</v>
@@ -1594,7 +1723,7 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D34">
         <v>0.7899999999999999</v>
@@ -1623,7 +1752,7 @@
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D35">
         <v>0.74</v>
@@ -1652,7 +1781,7 @@
         <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D36">
         <v>0.76</v>
@@ -1681,7 +1810,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D37">
         <v>0.9099999999999999</v>
@@ -1710,7 +1839,7 @@
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D38">
         <v>0.7899999999999999</v>
@@ -1739,7 +1868,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D39">
         <v>0.96</v>
@@ -1768,7 +1897,7 @@
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D40">
         <v>0.991</v>
@@ -1797,7 +1926,7 @@
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D41">
         <v>0.994</v>
@@ -1826,7 +1955,7 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D42">
         <v>0.998</v>
@@ -1855,7 +1984,7 @@
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D43">
         <v>0.998</v>
@@ -1884,7 +2013,7 @@
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D44">
         <v>0.8099999999999999</v>
@@ -1913,7 +2042,7 @@
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D45">
         <v>0.8999999999999999</v>
@@ -1942,7 +2071,7 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D46">
         <v>0.9819999999999999</v>
@@ -1971,7 +2100,7 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D47">
         <v>0.87</v>
@@ -2000,7 +2129,7 @@
         <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D48">
         <v>0.6999999999999998</v>
@@ -2029,7 +2158,7 @@
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D49">
         <v>0.9499999999999998</v>
@@ -2058,7 +2187,7 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D50">
         <v>0.993</v>
@@ -2087,7 +2216,7 @@
         <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D51">
         <v>0.89</v>
@@ -2116,7 +2245,7 @@
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D52">
         <v>0.7600000000000001</v>
@@ -2145,7 +2274,7 @@
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D53">
         <v>0.7200000000000001</v>
@@ -2174,7 +2303,7 @@
         <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D54">
         <v>0.9099999999999998</v>
@@ -2203,7 +2332,7 @@
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D55">
         <v>0.9099999999999998</v>
@@ -2232,7 +2361,7 @@
         <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D56">
         <v>0.93</v>
@@ -2261,7 +2390,7 @@
         <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D57">
         <v>0.9399999999999999</v>
@@ -2290,7 +2419,7 @@
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D58">
         <v>0.987</v>
@@ -2319,7 +2448,7 @@
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D59">
         <v>0.8899999999999999</v>
@@ -2348,7 +2477,7 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D60">
         <v>0.9299999999999999</v>
@@ -2377,7 +2506,7 @@
         <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D61">
         <v>0.9399999999999998</v>
@@ -2406,7 +2535,7 @@
         <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D62">
         <v>0.8899999999999999</v>
@@ -2435,7 +2564,7 @@
         <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D63">
         <v>0.9299999999999999</v>
@@ -2464,7 +2593,7 @@
         <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D64">
         <v>0.96</v>
@@ -2493,7 +2622,7 @@
         <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D65">
         <v>0.96</v>
@@ -2522,7 +2651,7 @@
         <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D66">
         <v>0.982</v>
@@ -2551,7 +2680,7 @@
         <v>13</v>
       </c>
       <c r="C67" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D67">
         <v>0.74</v>
@@ -2580,7 +2709,7 @@
         <v>13</v>
       </c>
       <c r="C68" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D68">
         <v>0.8699999999999999</v>
@@ -2609,7 +2738,7 @@
         <v>13</v>
       </c>
       <c r="C69" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D69">
         <v>0.9199999999999999</v>
@@ -2638,7 +2767,7 @@
         <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D70">
         <v>0.9800000000000001</v>
@@ -2667,7 +2796,7 @@
         <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D71">
         <v>0.96</v>
@@ -2696,7 +2825,7 @@
         <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D72">
         <v>0.95</v>
@@ -2717,8 +2846,1168 @@
         <v>6</v>
       </c>
     </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" t="s">
+        <v>88</v>
+      </c>
+      <c r="D73">
+        <v>0.984</v>
+      </c>
+      <c r="E73">
+        <v>0.1847239980152887</v>
+      </c>
+      <c r="F73">
+        <v>0.955</v>
+      </c>
+      <c r="G73">
+        <v>0.6489001692047377</v>
+      </c>
+      <c r="H73">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="I73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" t="s">
+        <v>89</v>
+      </c>
+      <c r="D74">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="E74">
+        <v>0.5071829918124481</v>
+      </c>
+      <c r="F74">
+        <v>0.98</v>
+      </c>
+      <c r="G74">
+        <v>0.8257191201353637</v>
+      </c>
+      <c r="H74">
+        <v>0.5</v>
+      </c>
+      <c r="I74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" t="s">
+        <v>90</v>
+      </c>
+      <c r="D75">
+        <v>0.77</v>
+      </c>
+      <c r="E75">
+        <v>0.6615905245346869</v>
+      </c>
+      <c r="F75">
+        <v>0.99</v>
+      </c>
+      <c r="G75">
+        <v>0.8307952622673435</v>
+      </c>
+      <c r="H75">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="I75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76" t="s">
+        <v>91</v>
+      </c>
+      <c r="D76">
+        <v>0.93</v>
+      </c>
+      <c r="E76">
+        <v>0.6615905245346869</v>
+      </c>
+      <c r="F76">
+        <v>0.99</v>
+      </c>
+      <c r="G76">
+        <v>0.8307952622673435</v>
+      </c>
+      <c r="H76">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="I76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" t="s">
+        <v>92</v>
+      </c>
+      <c r="D77">
+        <v>0.9979999999999999</v>
+      </c>
+      <c r="E77">
+        <v>0.5744416851006197</v>
+      </c>
+      <c r="F77">
+        <v>0.99</v>
+      </c>
+      <c r="G77">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="H77">
+        <v>0.5</v>
+      </c>
+      <c r="I77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78">
+        <v>0.7899999999999999</v>
+      </c>
+      <c r="E78">
+        <v>0.701702064128381</v>
+      </c>
+      <c r="F78">
+        <v>0.985</v>
+      </c>
+      <c r="G78">
+        <v>0.9923857868020305</v>
+      </c>
+      <c r="H78">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="I78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79">
+        <v>0.8099999999999999</v>
+      </c>
+      <c r="E79">
+        <v>0.5700066912114538</v>
+      </c>
+      <c r="F79">
+        <v>0.985</v>
+      </c>
+      <c r="G79">
+        <v>0.8282571912013537</v>
+      </c>
+      <c r="H79">
+        <v>0.5714285714285715</v>
+      </c>
+      <c r="I79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80" t="s">
+        <v>95</v>
+      </c>
+      <c r="D80">
+        <v>0.82</v>
+      </c>
+      <c r="E80">
+        <v>0.7706546758708627</v>
+      </c>
+      <c r="F80">
+        <v>0.99</v>
+      </c>
+      <c r="G80">
+        <v>0.9949238578680203</v>
+      </c>
+      <c r="H80">
+        <v>0.7499999999999999</v>
+      </c>
+      <c r="I80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" t="s">
+        <v>96</v>
+      </c>
+      <c r="D81">
+        <v>0.999</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0.985</v>
+      </c>
+      <c r="G81">
+        <v>0.5</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82" t="s">
+        <v>97</v>
+      </c>
+      <c r="D82">
+        <v>0.9099999999999998</v>
+      </c>
+      <c r="E82">
+        <v>0.8144321109212623</v>
+      </c>
+      <c r="F82">
+        <v>0.995</v>
+      </c>
+      <c r="G82">
+        <v>0.8333333333333333</v>
+      </c>
+      <c r="H82">
+        <v>0.8</v>
+      </c>
+      <c r="I82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" t="s">
+        <v>98</v>
+      </c>
+      <c r="D83">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="E83">
+        <v>0.8144321109212623</v>
+      </c>
+      <c r="F83">
+        <v>0.995</v>
+      </c>
+      <c r="G83">
+        <v>0.8333333333333333</v>
+      </c>
+      <c r="H83">
+        <v>0.8</v>
+      </c>
+      <c r="I83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" t="s">
+        <v>99</v>
+      </c>
+      <c r="D84">
+        <v>0.9700000000000001</v>
+      </c>
+      <c r="E84">
+        <v>0.6615905245346869</v>
+      </c>
+      <c r="F84">
+        <v>0.99</v>
+      </c>
+      <c r="G84">
+        <v>0.8307952622673435</v>
+      </c>
+      <c r="H84">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="I84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" t="s">
+        <v>100</v>
+      </c>
+      <c r="D85">
+        <v>0.995</v>
+      </c>
+      <c r="E85">
+        <v>0.8144321109212623</v>
+      </c>
+      <c r="F85">
+        <v>0.995</v>
+      </c>
+      <c r="G85">
+        <v>0.8333333333333333</v>
+      </c>
+      <c r="H85">
+        <v>0.8</v>
+      </c>
+      <c r="I85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" t="s">
+        <v>101</v>
+      </c>
+      <c r="D86">
+        <v>0.9899999999999999</v>
+      </c>
+      <c r="E86">
+        <v>0.6615905245346869</v>
+      </c>
+      <c r="F86">
+        <v>0.99</v>
+      </c>
+      <c r="G86">
+        <v>0.8307952622673435</v>
+      </c>
+      <c r="H86">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="I86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" t="s">
+        <v>102</v>
+      </c>
+      <c r="D87">
+        <v>0.981</v>
+      </c>
+      <c r="E87">
+        <v>0.8638245732792135</v>
+      </c>
+      <c r="F87">
+        <v>0.995</v>
+      </c>
+      <c r="G87">
+        <v>0.875</v>
+      </c>
+      <c r="H87">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" t="s">
+        <v>103</v>
+      </c>
+      <c r="D88">
+        <v>0.9099999999999999</v>
+      </c>
+      <c r="E88">
+        <v>0.7448979591836735</v>
+      </c>
+      <c r="F88">
+        <v>0.99</v>
+      </c>
+      <c r="G88">
+        <v>0.8724489795918368</v>
+      </c>
+      <c r="H88">
+        <v>0.75</v>
+      </c>
+      <c r="I88">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" t="s">
+        <v>104</v>
+      </c>
+      <c r="D89">
+        <v>0.992</v>
+      </c>
+      <c r="E89">
+        <v>0.8638245732792135</v>
+      </c>
+      <c r="F89">
+        <v>0.995</v>
+      </c>
+      <c r="G89">
+        <v>0.875</v>
+      </c>
+      <c r="H89">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" t="s">
+        <v>105</v>
+      </c>
+      <c r="D90">
+        <v>0.989</v>
+      </c>
+      <c r="E90">
+        <v>0.8638245732792135</v>
+      </c>
+      <c r="F90">
+        <v>0.995</v>
+      </c>
+      <c r="G90">
+        <v>0.875</v>
+      </c>
+      <c r="H90">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" t="s">
+        <v>106</v>
+      </c>
+      <c r="D91">
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="E91">
+        <v>0.8123201004396181</v>
+      </c>
+      <c r="F91">
+        <v>0.99</v>
+      </c>
+      <c r="G91">
+        <v>0.9948979591836735</v>
+      </c>
+      <c r="H91">
+        <v>0.8</v>
+      </c>
+      <c r="I91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" t="s">
+        <v>107</v>
+      </c>
+      <c r="D92">
+        <v>0.983</v>
+      </c>
+      <c r="E92">
+        <v>0.8638245732792135</v>
+      </c>
+      <c r="F92">
+        <v>0.995</v>
+      </c>
+      <c r="G92">
+        <v>0.875</v>
+      </c>
+      <c r="H92">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" t="s">
+        <v>108</v>
+      </c>
+      <c r="D93">
+        <v>0.996</v>
+      </c>
+      <c r="E93">
+        <v>0.8638245732792135</v>
+      </c>
+      <c r="F93">
+        <v>0.995</v>
+      </c>
+      <c r="G93">
+        <v>0.875</v>
+      </c>
+      <c r="H93">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" t="s">
+        <v>109</v>
+      </c>
+      <c r="D94">
+        <v>0.994</v>
+      </c>
+      <c r="E94">
+        <v>0.8638245732792135</v>
+      </c>
+      <c r="F94">
+        <v>0.995</v>
+      </c>
+      <c r="G94">
+        <v>0.875</v>
+      </c>
+      <c r="H94">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I94">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" t="s">
+        <v>110</v>
+      </c>
+      <c r="D95">
+        <v>0.87</v>
+      </c>
+      <c r="E95">
+        <v>0.8638245732792135</v>
+      </c>
+      <c r="F95">
+        <v>0.995</v>
+      </c>
+      <c r="G95">
+        <v>0.875</v>
+      </c>
+      <c r="H95">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" t="s">
+        <v>111</v>
+      </c>
+      <c r="D96">
+        <v>0.86</v>
+      </c>
+      <c r="E96">
+        <v>0.8638245732792135</v>
+      </c>
+      <c r="F96">
+        <v>0.995</v>
+      </c>
+      <c r="G96">
+        <v>0.875</v>
+      </c>
+      <c r="H96">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" t="s">
+        <v>112</v>
+      </c>
+      <c r="D97">
+        <v>0.993</v>
+      </c>
+      <c r="E97">
+        <v>0.8638245732792135</v>
+      </c>
+      <c r="F97">
+        <v>0.995</v>
+      </c>
+      <c r="G97">
+        <v>0.875</v>
+      </c>
+      <c r="H97">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" t="s">
+        <v>113</v>
+      </c>
+      <c r="D98">
+        <v>0.994</v>
+      </c>
+      <c r="E98">
+        <v>0.8638245732792135</v>
+      </c>
+      <c r="F98">
+        <v>0.995</v>
+      </c>
+      <c r="G98">
+        <v>0.875</v>
+      </c>
+      <c r="H98">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" t="s">
+        <v>114</v>
+      </c>
+      <c r="D99">
+        <v>0.997</v>
+      </c>
+      <c r="E99">
+        <v>0.7448979591836735</v>
+      </c>
+      <c r="F99">
+        <v>0.99</v>
+      </c>
+      <c r="G99">
+        <v>0.8724489795918368</v>
+      </c>
+      <c r="H99">
+        <v>0.75</v>
+      </c>
+      <c r="I99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" t="s">
+        <v>115</v>
+      </c>
+      <c r="D100">
+        <v>0.995</v>
+      </c>
+      <c r="E100">
+        <v>0.7448979591836735</v>
+      </c>
+      <c r="F100">
+        <v>0.99</v>
+      </c>
+      <c r="G100">
+        <v>0.8724489795918368</v>
+      </c>
+      <c r="H100">
+        <v>0.75</v>
+      </c>
+      <c r="I100">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>16</v>
+      </c>
+      <c r="C101" t="s">
+        <v>116</v>
+      </c>
+      <c r="D101">
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="E101">
+        <v>0.7706546758708627</v>
+      </c>
+      <c r="F101">
+        <v>0.99</v>
+      </c>
+      <c r="G101">
+        <v>0.8</v>
+      </c>
+      <c r="H101">
+        <v>0.7499999999999999</v>
+      </c>
+      <c r="I101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" t="s">
+        <v>117</v>
+      </c>
+      <c r="D102">
+        <v>0.982</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>1</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>16</v>
+      </c>
+      <c r="C103" t="s">
+        <v>118</v>
+      </c>
+      <c r="D103">
+        <v>0.984</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>16</v>
+      </c>
+      <c r="C104" t="s">
+        <v>119</v>
+      </c>
+      <c r="D104">
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="E104">
+        <v>0.910527225875113</v>
+      </c>
+      <c r="F104">
+        <v>0.995</v>
+      </c>
+      <c r="G104">
+        <v>0.9974358974358974</v>
+      </c>
+      <c r="H104">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="I104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105" t="s">
+        <v>120</v>
+      </c>
+      <c r="D105">
+        <v>0.99</v>
+      </c>
+      <c r="E105">
+        <v>0.910527225875113</v>
+      </c>
+      <c r="F105">
+        <v>0.995</v>
+      </c>
+      <c r="G105">
+        <v>0.9974358974358974</v>
+      </c>
+      <c r="H105">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="I105">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>16</v>
+      </c>
+      <c r="C106" t="s">
+        <v>121</v>
+      </c>
+      <c r="D106">
+        <v>0.991</v>
+      </c>
+      <c r="E106">
+        <v>0.910527225875113</v>
+      </c>
+      <c r="F106">
+        <v>0.995</v>
+      </c>
+      <c r="G106">
+        <v>0.9974358974358974</v>
+      </c>
+      <c r="H106">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="I106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>16</v>
+      </c>
+      <c r="C107" t="s">
+        <v>122</v>
+      </c>
+      <c r="D107">
+        <v>0.9099999999999999</v>
+      </c>
+      <c r="E107">
+        <v>0.7706546758708627</v>
+      </c>
+      <c r="F107">
+        <v>0.99</v>
+      </c>
+      <c r="G107">
+        <v>0.8</v>
+      </c>
+      <c r="H107">
+        <v>0.7499999999999999</v>
+      </c>
+      <c r="I107">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>16</v>
+      </c>
+      <c r="C108" t="s">
+        <v>123</v>
+      </c>
+      <c r="D108">
+        <v>0.9890000000000001</v>
+      </c>
+      <c r="E108">
+        <v>0.910527225875113</v>
+      </c>
+      <c r="F108">
+        <v>0.995</v>
+      </c>
+      <c r="G108">
+        <v>0.9974358974358974</v>
+      </c>
+      <c r="H108">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="I108">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>16</v>
+      </c>
+      <c r="C109" t="s">
+        <v>124</v>
+      </c>
+      <c r="D109">
+        <v>0.9949999999999999</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109">
+        <v>1</v>
+      </c>
+      <c r="G109">
+        <v>1</v>
+      </c>
+      <c r="H109">
+        <v>1</v>
+      </c>
+      <c r="I109">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110" t="s">
+        <v>125</v>
+      </c>
+      <c r="D110">
+        <v>0.998</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+      <c r="G110">
+        <v>1</v>
+      </c>
+      <c r="H110">
+        <v>1</v>
+      </c>
+      <c r="I110">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>16</v>
+      </c>
+      <c r="C111" t="s">
+        <v>126</v>
+      </c>
+      <c r="D111">
+        <v>0.998</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>1</v>
+      </c>
+      <c r="G111">
+        <v>1</v>
+      </c>
+      <c r="H111">
+        <v>1</v>
+      </c>
+      <c r="I111">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>16</v>
+      </c>
+      <c r="C112" t="s">
+        <v>127</v>
+      </c>
+      <c r="D112">
+        <v>0.9960000000000001</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <v>1</v>
+      </c>
+      <c r="G112">
+        <v>1</v>
+      </c>
+      <c r="H112">
+        <v>1</v>
+      </c>
+      <c r="I112">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E72">
+  <conditionalFormatting sqref="E2:E112">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2730,7 +4019,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F72">
+  <conditionalFormatting sqref="F2:F112">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2742,7 +4031,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G72">
+  <conditionalFormatting sqref="G2:G112">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2754,7 +4043,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H72">
+  <conditionalFormatting sqref="H2:H112">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>